<commit_message>
added file for 5th month
</commit_message>
<xml_diff>
--- a/Wastes/Month 3/month_3_wastes.xlsx
+++ b/Wastes/Month 3/month_3_wastes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Lunches" sheetId="1" r:id="rId1"/>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,9 +624,21 @@
       <c r="D5">
         <v>6.9</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>5.3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="I5">
         <f xml:space="preserve"> B5+C5+D5+E5+F5+G5+H5</f>
-        <v>9.3000000000000007</v>
+        <v>14.600000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,7 +647,7 @@
       </c>
       <c r="I6">
         <f xml:space="preserve"> I2+I3+I4+I5</f>
-        <v>48.8</v>
+        <v>54.1</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -1537,7 +1549,7 @@
       </c>
       <c r="B2">
         <f xml:space="preserve"> Lunches!I6</f>
-        <v>48.8</v>
+        <v>54.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1582,7 +1594,7 @@
       </c>
       <c r="B7">
         <f xml:space="preserve"> B2+B3+B5+B6</f>
-        <v>461.70000000000005</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>